<commit_message>
debugged duplication and fixed api issue
</commit_message>
<xml_diff>
--- a/files/Final_Report.xlsx
+++ b/files/Final_Report.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,8 +475,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="24" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
-    <col width="26" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -487,11 +490,14 @@
       </c>
       <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
     </row>
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-04</t>
         </is>
       </c>
     </row>
@@ -499,15 +505,30 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>Comapany</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
           <t>Account</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>Document currency</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>Amount in doc. curr.</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Local Currency</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>Amount in local currency</t>
         </is>
@@ -516,266 +537,566 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>UN0100</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>63010001</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>-6850603.8</v>
       </c>
-      <c r="C5" t="n">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
         <v>-6850603.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>63010002</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>11501418.04</v>
       </c>
-      <c r="C6" t="n">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
         <v>11501418.04</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>63010011</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>-1479775595.78</v>
       </c>
-      <c r="C7" t="n">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
         <v>-7946810.529999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>UN0150</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>63010012</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>1495088917.7</v>
       </c>
-      <c r="C8" t="n">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
         <v>8028294.79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>63010061</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>HKD</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>-1800000</v>
       </c>
-      <c r="C9" t="n">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
         <v>-232183.17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>63010101</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>-41779.00999999999</v>
       </c>
-      <c r="C10" t="n">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
         <v>-46504.21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>UN0100</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>63010162</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>1354247.56</v>
       </c>
-      <c r="C11" t="n">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
         <v>1354247.56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>UN0150</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>63010502</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>1368805.95</v>
       </c>
-      <c r="C12" t="n">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
         <v>1368805.95</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>63011001</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>-506397.46</v>
       </c>
-      <c r="C13" t="n">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
         <v>-506397.46</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>63011011</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>-181229989.54</v>
       </c>
-      <c r="C14" t="n">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
         <v>-973255.86</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>XT0151</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>63020001</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>-3354998.88</v>
       </c>
-      <c r="C15" t="n">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>-18017.3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>63020002</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>3533034.32</v>
       </c>
-      <c r="C16" t="n">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
         <v>18973.41</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>63020051</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>-29242804.73</v>
       </c>
-      <c r="C17" t="n">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
         <v>-157042.07</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>UN0100</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>63020602</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
         <v>13969885.84</v>
       </c>
-      <c r="C18" t="n">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
         <v>75022.22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>UN0150</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>63020621</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>-4375</v>
       </c>
-      <c r="C19" t="n">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
         <v>-4375</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>63070001</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
         <v>-2532414</v>
       </c>
-      <c r="C20" t="n">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
         <v>-2532414</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>XT0150</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>63070002</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
         <v>2853277.16</v>
       </c>
-      <c r="C21" t="n">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
         <v>2853277.16</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>UN0150</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>63070012</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
         <v>250851.46</v>
       </c>
-      <c r="C22" t="n">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
         <v>250851.46</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>UN0150</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>63070501</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>-301238357.4</v>
       </c>
-      <c r="C23" t="n">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
         <v>-1617734.58</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>UN0150</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>63070502</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>LKR</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>398347604.24</v>
       </c>
-      <c r="C24" t="n">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
         <v>2139238.51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>